<commit_message>
fix distance estimation equation, add data
</commit_message>
<xml_diff>
--- a/Lab2_distancesensor/SensorCalibration.xlsx
+++ b/Lab2_distancesensor/SensorCalibration.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Distance (in)</t>
   </si>
@@ -162,11 +162,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$2</c:f>
+              <c:f>Sheet1!$B$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Analog Reading</c:v>
+                  <c:v>Distance (in)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -192,7 +192,40 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$3:$A$10</c:f>
+              <c:f>Sheet1!$A$13:$A$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>199</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>217</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>243</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>287</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>329</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>468</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>496</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>571</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$13:$B$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -219,39 +252,6 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>7.5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$3:$B$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>199</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>217</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>243</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>287</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>329</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>468</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>496</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>571</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -266,11 +266,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="625042560"/>
-        <c:axId val="625043136"/>
+        <c:axId val="87664896"/>
+        <c:axId val="87665472"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="625042560"/>
+        <c:axId val="87664896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -280,12 +280,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="625043136"/>
+        <c:crossAx val="87665472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="625043136"/>
+        <c:axId val="87665472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -296,7 +296,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="625042560"/>
+        <c:crossAx val="87664896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -640,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -831,6 +831,79 @@
       </c>
       <c r="B10" s="2">
         <v>571</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>199</v>
+      </c>
+      <c r="B13" s="2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>217</v>
+      </c>
+      <c r="B14" s="2">
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>243</v>
+      </c>
+      <c r="B15" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>287</v>
+      </c>
+      <c r="B16" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>329</v>
+      </c>
+      <c r="B17" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>468</v>
+      </c>
+      <c r="B18" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>496</v>
+      </c>
+      <c r="B19" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>571</v>
+      </c>
+      <c r="B20" s="2">
+        <v>7.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>